<commit_message>
Subindo alterações no PBC e documentação
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos/PBC - Product Backlog Classified V2.xlsx
+++ b/Documentação/Gráficos/PBC - Product Backlog Classified V2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\SPRINT2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8749434A-3DD8-4284-BDF8-392382EAD981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68F26846-AAEB-45BF-B679-22FF4B890BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SB" sheetId="16" r:id="rId2"/>
     <sheet name="Dados" sheetId="14" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,31 +39,6 @@
     <author>Alexander Barreira</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{CDAF273E-A20B-4D5C-B0D1-B3564A967A64}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexander Barreira:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Preencher com a  Sigla do Artefato#o Número (ID) do requisito e o &lt;Grupo ao qual o Requisito faz parte&gt;
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E4" authorId="0" shapeId="0" xr:uid="{EE39FC19-3292-4006-90AF-BA8C8E76E8E0}">
       <text>
         <r>
@@ -94,312 +69,387 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="127">
+  <si>
+    <t>Product BackLog Classified (PBC)</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Artefato de Referência (XX#R)</t>
+  </si>
+  <si>
+    <t>Descrição do Requisito</t>
+  </si>
+  <si>
+    <t>Pontos</t>
+  </si>
+  <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Desejavél</t>
+  </si>
+  <si>
+    <t>Planejada</t>
+  </si>
+  <si>
+    <t>US#1 &lt;Cadastro&gt;</t>
+  </si>
+  <si>
+    <t>O sistema deve ter um cadastro de locador</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>US#1 &lt;usabilidade/UX&gt;</t>
+  </si>
+  <si>
+    <t>O Sistemas deverá ter um filtro especifico para cada periodo de aluguel (diária, semanal, mensal)</t>
+  </si>
+  <si>
+    <t>US#1&lt;usabilidade/UX&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O Sistema deverá ter um filtro de disponibilidade por data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deverá filtrar os imóveis por valor selecionado </t>
+  </si>
+  <si>
+    <t>US#2&lt;usabilidade&gt;</t>
+  </si>
+  <si>
+    <t>O sistema deverá ter um formulário para criação de anuncio dos imóveis</t>
+  </si>
+  <si>
+    <t>US#2&lt;usabilidade/UX&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O formulário de anuncio de imóveis deverá ter um calendario para marcar os periodos disponíveis </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>US#3&lt;anuncio&gt;</t>
+  </si>
+  <si>
+    <t>O formulário de anuncio de imóveis deverá ter um campo de matricula do imóvel</t>
+  </si>
+  <si>
+    <t>US#3&lt;validação&gt;</t>
+  </si>
+  <si>
+    <t>O sistema deverá validar se o campo de matricula foi inserido ou se já existe</t>
+  </si>
+  <si>
+    <t>US#4&lt;anuncio&gt;</t>
+  </si>
+  <si>
+    <t>O formulário de anuncio de imóvel deverá ter a opção para upload de imagens</t>
+  </si>
+  <si>
+    <t>US#4&lt;validação&gt;</t>
+  </si>
+  <si>
+    <t>O formulário de anuncio de imóvel deverá ter  pelo menos uma imagem upada para ser validado</t>
+  </si>
+  <si>
+    <t>US#5&lt;usabilidade/UX&gt;</t>
+  </si>
+  <si>
+    <t>O formulário de anuncio de imóvel deverá estar separado por etapas para facilitar o preenchimento</t>
+  </si>
+  <si>
+    <t>O formulário de anuncio de imóvel deverá ter mascara em todos os input's</t>
+  </si>
+  <si>
+    <t>O formulário de anuncio de imóvel deverá conter textos de auto ajuda para o preenchimento dos campos</t>
+  </si>
+  <si>
+    <t>US#6&lt;simulador&gt;</t>
+  </si>
+  <si>
+    <t>O sistema deverá ter um simulador de valores para cada modalidade de aluguel</t>
+  </si>
+  <si>
+    <t>O simulador financeiro deverá ter a opção de simular pela quantidade de (dias/semanas/meses)</t>
+  </si>
+  <si>
+    <t>US#7&lt;avaliação de anuncio&gt;</t>
+  </si>
+  <si>
+    <t>O sistema deverá ter um sistema de avaliação nos anúncios</t>
+  </si>
+  <si>
+    <t>O sistema deverá ter um post de comentarios em cada anúncio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deverar ter uma avaliação com rank de estrelas de 1 a 5 para cada anuncio </t>
+  </si>
+  <si>
+    <t>O sistema deverar exibir a média de estrelas em cada anúncio</t>
+  </si>
+  <si>
+    <t>US#8&lt;Gráfico de GANTT&gt;</t>
+  </si>
+  <si>
+    <t>US#9&lt;Product/Sprint Backlog&gt;</t>
+  </si>
+  <si>
+    <t>US#10&lt;Modelagem de Dados​&gt;</t>
+  </si>
+  <si>
+    <t>US#11Planilha de Arquitetura&gt;</t>
+  </si>
+  <si>
+    <t>US#12&lt;Diagrama de Solução de Software&gt;</t>
+  </si>
+  <si>
+    <t>US#13&lt;Interface WEB com regras de usabilidade&gt;</t>
+  </si>
+  <si>
+    <t>US#14&lt;2 CRUDs (SpringBoot + ORM)&gt;</t>
+  </si>
+  <si>
+    <t>Implementar e integrar nos Cruds</t>
+  </si>
+  <si>
+    <t>US#15&lt;Login/LogOff com ORM&gt;</t>
+  </si>
+  <si>
+    <t>Realizar o processo de logon com ORM</t>
+  </si>
+  <si>
+    <t>US#16&lt;Funcionalidade de exportação de arquivos&gt;</t>
+  </si>
+  <si>
+    <t>US#17&lt;Documento de Layout (Entrada e Saída)&gt;</t>
+  </si>
+  <si>
+    <t>Montar e estruturar o Layout</t>
+  </si>
+  <si>
+    <t>US#18&lt;Implementação de lista&gt;</t>
+  </si>
+  <si>
+    <t>US#19&lt;Padrão de projeto (2 tipos)​&gt;</t>
+  </si>
+  <si>
+    <t>Tarefa principal</t>
+  </si>
+  <si>
+    <t>Descrição da tarefa</t>
+  </si>
+  <si>
+    <t>Gráfico de GANTT</t>
+  </si>
+  <si>
+    <t>N° Fibonacci</t>
+  </si>
+  <si>
+    <t>Product/Sprint Backlog</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 2, 3, 5, 8, 13, 21</t>
+  </si>
+  <si>
+    <t>Modelagem de Dados​</t>
+  </si>
+  <si>
+    <t>Planilha de Arquitetura</t>
+  </si>
+  <si>
+    <t>Diagrama de Solução de Software</t>
+  </si>
+  <si>
+    <t>Interface WEB com regras de usabilidade</t>
+  </si>
+  <si>
+    <t>2 CRUDs (SpringBoot + ORM)</t>
+  </si>
+  <si>
+    <t>Login/LogOff com ORM</t>
+  </si>
+  <si>
+    <t>Funcionalidade de exportação de arquivos</t>
+  </si>
+  <si>
+    <t>Documento de Layout (Entrada e Saída)</t>
+  </si>
+  <si>
+    <t>Implementação de lista</t>
+  </si>
+  <si>
+    <t>Padrão de projeto (2 tipos)​</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Cancelado</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>Congelada</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
   <si>
     <t>∞</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
-    <t>Desejavél</t>
-  </si>
-  <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <t>Descrição do Requisito</t>
-  </si>
-  <si>
-    <t>Pontos</t>
-  </si>
-  <si>
-    <t>US#1 &lt;Cadastro&gt;</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Feito</t>
-  </si>
-  <si>
-    <t>Cancelado</t>
-  </si>
-  <si>
-    <t>Em Andamento</t>
-  </si>
-  <si>
-    <t>Planejada</t>
-  </si>
-  <si>
-    <t>Congelada</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Product BackLog Classified (PBC)</t>
+    <t xml:space="preserve">Artefato (ferramenta) </t>
+  </si>
+  <si>
+    <t>sigla</t>
   </si>
   <si>
     <t>BPMN</t>
   </si>
   <si>
+    <t>BP</t>
+  </si>
+  <si>
     <t xml:space="preserve">PROTOTIPO DE TELA </t>
   </si>
   <si>
+    <t>PT</t>
+  </si>
+  <si>
     <t>USER STORIES</t>
   </si>
   <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>CANVAS</t>
   </si>
   <si>
+    <t>CC</t>
+  </si>
+  <si>
     <t>STORIE BOARD</t>
   </si>
   <si>
+    <t>SB</t>
+  </si>
+  <si>
     <t>MAPA DE EMPATIA</t>
   </si>
   <si>
+    <t>ME</t>
+  </si>
+  <si>
     <t>DESENHO DE ARQUITETURA</t>
   </si>
   <si>
+    <t>DE</t>
+  </si>
+  <si>
     <t>JORNADA DO USUÁRIO</t>
   </si>
   <si>
+    <t>JU</t>
+  </si>
+  <si>
     <t xml:space="preserve">DER </t>
   </si>
   <si>
-    <t>PT</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>SB</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>JU</t>
-  </si>
-  <si>
     <t>DR</t>
   </si>
   <si>
+    <t>USE CASE</t>
+  </si>
+  <si>
     <t>UC</t>
   </si>
   <si>
-    <t>USE CASE</t>
-  </si>
-  <si>
-    <t>BP</t>
-  </si>
-  <si>
-    <t>Artefato de Referência (XX#R)</t>
-  </si>
-  <si>
-    <t>sigla</t>
+    <t>ENTREVISTA DE CAMPO</t>
   </si>
   <si>
     <t>EC</t>
   </si>
   <si>
-    <t>ENTREVISTA DE CAMPO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artefato (ferramenta) </t>
-  </si>
-  <si>
-    <t>O Sistemas deverá ter um filtro especifico para cada periodo de aluguel (diária, semanal, mensal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O Sistema deverá ter um filtro de disponibilidade por data </t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deverá filtrar os imóveis por valor selecionado </t>
-  </si>
-  <si>
-    <t>US#1 &lt;usabilidade/UX&gt;</t>
-  </si>
-  <si>
-    <t>US#1&lt;usabilidade/UX&gt;</t>
-  </si>
-  <si>
-    <t>US#2&lt;usabilidade/UX&gt;</t>
-  </si>
-  <si>
-    <t>O sistema deverá ter um formulário para criação de anuncio dos imóveis</t>
-  </si>
-  <si>
-    <t>US#2&lt;usabilidade&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O formulário de anuncio de imóveis deverá ter um calendario para marcar os periodos disponíveis </t>
-  </si>
-  <si>
-    <t>US#3&lt;validação&gt;</t>
-  </si>
-  <si>
-    <t>US#3&lt;anuncio&gt;</t>
-  </si>
-  <si>
-    <t>US#4&lt;anuncio&gt;</t>
-  </si>
-  <si>
-    <t>O formulário de anuncio de imóvel deverá ter  pelo menos uma imagem upada para ser validado</t>
-  </si>
-  <si>
-    <t>US#5&lt;usabilidade/UX&gt;</t>
-  </si>
-  <si>
-    <t>US#4&lt;validação&gt;</t>
-  </si>
-  <si>
-    <t>O formulário de anuncio de imóvel deverá conter textos de auto ajuda para o preenchimento dos campos</t>
-  </si>
-  <si>
-    <t>US#6&lt;simulador&gt;</t>
-  </si>
-  <si>
-    <t>O sistema deverá ter um simulador de valores para cada modalidade de aluguel</t>
-  </si>
-  <si>
-    <t>O simulador financeiro deverá ter a opção de simular pela quantidade de (dias/semanas/meses)</t>
-  </si>
-  <si>
-    <t>US#7&lt;avaliação de anuncio&gt;</t>
-  </si>
-  <si>
-    <t>O sistema deverá ter um post de comentarios em cada anúncio</t>
-  </si>
-  <si>
-    <t>O sistema deverar exibir a média de estrelas em cada anúncio</t>
-  </si>
-  <si>
-    <t>O sistema deve ter um cadastro de locador</t>
-  </si>
-  <si>
-    <t>O formulário de anuncio de imóveis deverá ter um campo de matricula do imóvel</t>
-  </si>
-  <si>
-    <t>O sistema deverá validar se o campo de matricula foi inserido ou se já existe</t>
-  </si>
-  <si>
-    <t>O formulário de anuncio de imóvel deverá ter a opção para upload de imagens</t>
-  </si>
-  <si>
-    <t>O formulário de anuncio de imóvel deverá estar separado por etapas para facilitar o preenchimento</t>
-  </si>
-  <si>
-    <t>O formulário de anuncio de imóvel deverá ter mascara em todos os input's</t>
-  </si>
-  <si>
-    <t>O sistema deverá ter um sistema de avaliação nos anúncios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deverar ter uma avaliação com rank de estrelas de 1 a 5 para cada anuncio </t>
-  </si>
-  <si>
-    <t>0, 1, 1, 2, 3, 5, 8, 13, 21</t>
-  </si>
-  <si>
-    <t>N° Fibonacci</t>
-  </si>
-  <si>
-    <t>Tarefa principal</t>
-  </si>
-  <si>
-    <t>Descrição da tarefa</t>
-  </si>
-  <si>
-    <t>User Story</t>
-  </si>
-  <si>
-    <t>Gráfico de GANTT</t>
-  </si>
-  <si>
-    <t>Product/Sprint Backlog</t>
-  </si>
-  <si>
-    <t>Modelagem de Dados​</t>
-  </si>
-  <si>
-    <t>Planilha de Arquitetura</t>
-  </si>
-  <si>
-    <t>Diagrama de Solução de Software</t>
-  </si>
-  <si>
-    <t>Interface WEB com regras de usabilidade</t>
-  </si>
-  <si>
-    <t>2 CRUDs (SpringBoot + ORM)</t>
-  </si>
-  <si>
-    <t>Login/LogOff com ORM</t>
-  </si>
-  <si>
-    <t>Funcionalidade de exportação de arquivos</t>
-  </si>
-  <si>
-    <t>Documento de Layout (Entrada e Saída)</t>
-  </si>
-  <si>
-    <t>Implementação de lista</t>
-  </si>
-  <si>
-    <t>Padrão de projeto (2 tipos)​</t>
-  </si>
-  <si>
-    <t>Separar as atividades em niveis de relevância</t>
-  </si>
-  <si>
-    <t>Criar as tabelas e realizar a implementação</t>
-  </si>
-  <si>
-    <t>Estruturar planilha de arquitetura</t>
-  </si>
-  <si>
-    <t>Fazer diagrama da solução de software</t>
-  </si>
-  <si>
-    <t>Acrescentar as regras na interface</t>
-  </si>
-  <si>
-    <t>Implementar e integrar nos Cruds</t>
-  </si>
-  <si>
-    <t>Realizar o processo de logon com ORM</t>
-  </si>
-  <si>
-    <t>Fazer com auxilio do CSV</t>
-  </si>
-  <si>
-    <t>Montar e estrturar o Layout</t>
-  </si>
-  <si>
-    <t>Usar lista no projeto</t>
-  </si>
-  <si>
-    <t>Escolher o padrão de projeto que melhor nos atende</t>
-  </si>
-  <si>
-    <t>Gráfico de evolução do projeto</t>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Gráfico de evolução e andamento do projeto</t>
+  </si>
+  <si>
+    <t>Separar as atividades em niveis de relevância e prioridade</t>
+  </si>
+  <si>
+    <t>Criar as tabelas e realizar a implementação no DER</t>
+  </si>
+  <si>
+    <t>Estruturar planilha de arquitetura seguindo o padrão</t>
+  </si>
+  <si>
+    <t>Fazer diagrama da solução de software seguindo os padrões estabelecidos</t>
+  </si>
+  <si>
+    <t>Acrescentar as regras na interface do projeto</t>
+  </si>
+  <si>
+    <t>Usar listas nas classes dentro do projeto</t>
+  </si>
+  <si>
+    <t>Escolher os padrões de projeto que melhor nos atende</t>
+  </si>
+  <si>
+    <t>Fazer com auxilio do CSV a exportação</t>
+  </si>
+  <si>
+    <t>Estruturar e montar o gráfico, atribuir atividades e colocar as fórmulas</t>
+  </si>
+  <si>
+    <t>Separar atividades, priorizar e coloca-lás em ordem</t>
+  </si>
+  <si>
+    <t>Estruturar o DER e implementar as classes</t>
+  </si>
+  <si>
+    <t>Montar a planilha e acrescentar os dados necessários</t>
+  </si>
+  <si>
+    <t>Fazer o diagrama seguindo a solução e arquitetura do projeto</t>
+  </si>
+  <si>
+    <t>Acrescentar e definir as regras de usabilidade</t>
+  </si>
+  <si>
+    <t>Implementar 2 Crud's com apoio do SpringBoot e ORM</t>
+  </si>
+  <si>
+    <t>Escolher os dois padrões de projeto: Observer e uma outra opção</t>
+  </si>
+  <si>
+    <t>Colocar listas nas classes dentro do projeto e implementar</t>
+  </si>
+  <si>
+    <t>Fazer seguindo o modelo e colocar dez dados como atributos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar ao código e exportar os arquivos que são necessários </t>
+  </si>
+  <si>
+    <t>Realizar o logon com ORM se adequando ao projeto</t>
   </si>
 </sst>
 </file>
@@ -409,7 +459,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -445,12 +495,6 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -526,23 +570,6 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color rgb="FFAE229D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="16"/>
-      <color rgb="FFAE229D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -557,6 +584,37 @@
     <font>
       <sz val="10"/>
       <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -601,12 +659,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -691,22 +749,123 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
       <right/>
-      <top/>
-      <bottom style="hair">
-        <color auto="1"/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="hair">
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,9 +892,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -754,7 +913,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -765,153 +924,300 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="4" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="21" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="21" builtinId="8"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2326,29 +2632,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="200.6640625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="0.6640625" style="21" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="24" customWidth="1"/>
-    <col min="8" max="11" width="20.6640625" style="22" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="22"/>
+    <col min="1" max="1" width="3.88671875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="200.6640625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="0.6640625" style="19" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="22" customWidth="1"/>
+    <col min="8" max="11" width="20.6640625" style="20" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:8" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="45" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -2358,474 +2664,557 @@
       <c r="H2" s="47"/>
     </row>
     <row r="3" spans="2:8" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:8" s="25" customFormat="1" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="33" t="s">
+    <row r="4" spans="2:8" s="23" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="2:8" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="2:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="25"/>
+    </row>
+    <row r="20" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="D20" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-    </row>
-    <row r="6" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="C21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="27"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="27"/>
-    </row>
-    <row r="7" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="D28" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="27"/>
-    </row>
-    <row r="9" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="D29" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="27"/>
+      <c r="F29" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="27"/>
+      <c r="F30" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+    </row>
+    <row r="31" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-    </row>
-    <row r="10" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="D31" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="E31" s="27"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="27"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="27"/>
-    </row>
-    <row r="12" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="27"/>
-    </row>
-    <row r="13" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="D33" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="27"/>
-    </row>
-    <row r="14" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="16" t="s">
+      <c r="E33" s="27"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="25"/>
+    </row>
+    <row r="34" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="2:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="D34" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="27"/>
+      <c r="F34" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+    </row>
+    <row r="35" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="27"/>
-    </row>
-    <row r="17" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="27"/>
-    </row>
-    <row r="19" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="27"/>
-    </row>
-    <row r="20" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-    </row>
-    <row r="26" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-    </row>
-    <row r="27" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-    </row>
-    <row r="30" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-    </row>
-    <row r="31" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-    </row>
-    <row r="33" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-    </row>
-    <row r="34" spans="2:8" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
+      <c r="D35" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="27"/>
+      <c r="F35" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2833,76 +3222,121 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B5:E5 C5:C6 B6:B34">
-    <cfRule type="expression" dxfId="20" priority="34">
+    <cfRule type="expression" dxfId="33" priority="47">
       <formula>$B5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="35">
+    <cfRule type="expression" dxfId="32" priority="48">
       <formula>$B5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="36">
+    <cfRule type="expression" dxfId="31" priority="49">
       <formula>$B5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="37">
+    <cfRule type="expression" dxfId="30" priority="50">
       <formula>$B5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="16" priority="26">
+    <cfRule type="expression" dxfId="29" priority="39">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="27">
+    <cfRule type="expression" dxfId="28" priority="40">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="28">
+    <cfRule type="expression" dxfId="27" priority="41">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="29">
+    <cfRule type="expression" dxfId="26" priority="42">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:E6">
-    <cfRule type="expression" dxfId="12" priority="18">
+    <cfRule type="expression" dxfId="25" priority="31">
       <formula>$B6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="19">
+    <cfRule type="expression" dxfId="24" priority="32">
       <formula>$B6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="20">
+    <cfRule type="expression" dxfId="23" priority="33">
       <formula>$B6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="21">
+    <cfRule type="expression" dxfId="22" priority="34">
       <formula>$B6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C34">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="20" priority="24">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="19" priority="25">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D34">
+    <cfRule type="expression" dxfId="17" priority="14">
+      <formula>$B$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="19">
+      <formula>$B8="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="20">
+      <formula>$B8="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="21">
+      <formula>$B8="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="22">
+      <formula>$B8="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>$B35="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>$B35="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>$B35="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="13">
+      <formula>$B35="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="8" priority="6">
+      <formula>$B35="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>$B35="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>$B35="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="9">
+      <formula>$B35="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>$B8="Done!"</formula>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$B35="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>$B8="Ongoing"</formula>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$B35="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>$B8="Blocked"</formula>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>$B35="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
-      <formula>$B8="Dropped"</formula>
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>$B35="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2919,13 +3353,13 @@
           <x14:formula1>
             <xm:f>Dados!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B34</xm:sqref>
+          <xm:sqref>B5:B35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Dados!$A$14:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E5 E7:E34</xm:sqref>
+          <xm:sqref>E5 E7:E35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2935,384 +3369,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F378867A-5387-429E-B87E-19913A3BDAD1}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" style="38" customWidth="1"/>
-    <col min="4" max="14" width="8.88671875" style="38"/>
-    <col min="15" max="15" width="21.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="38"/>
+    <col min="1" max="1" width="34.109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.5546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" style="31" customWidth="1"/>
+    <col min="4" max="14" width="8.88671875" style="31"/>
+    <col min="15" max="15" width="21.109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="37"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="O2" s="38" t="s">
-        <v>74</v>
+      <c r="A1" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="54">
+        <v>2</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="40"/>
-      <c r="O3" s="41" t="s">
-        <v>73</v>
+      <c r="A3" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="54">
+        <v>2</v>
+      </c>
+      <c r="O3" s="33" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="40"/>
+      <c r="A4" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="40"/>
+      <c r="A5" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="40"/>
+      <c r="A6" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="40"/>
+      <c r="A7" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="40"/>
+      <c r="A8" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="40"/>
+      <c r="A9" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="40"/>
+      <c r="A10" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="40"/>
+      <c r="A11" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="54">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="40"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="39"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="39"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="39"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="40"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="39"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="40"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="39"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="40"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="39"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="40"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="40"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="40"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="39"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="40"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="39"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="40"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="39"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="40"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="39"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="40"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="39"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="40"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="39"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="40"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="39"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="40"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="39"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="40"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="39"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="40"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="39"/>
-      <c r="B57" s="39"/>
-      <c r="C57" s="40"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="39"/>
-      <c r="B58" s="39"/>
-      <c r="C58" s="40"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="39"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="39"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="40"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="39"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="40"/>
+      <c r="A12" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="58">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3338,48 +3558,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>2</v>
+      <c r="A1" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="33.6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="H6" s="13" t="s">
-        <v>77</v>
+      <c r="H6" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3400,7 +3620,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
@@ -3408,105 +3628,105 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>38</v>
+      <c r="A16" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>17</v>
+      <c r="A17" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>18</v>
+      <c r="A18" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>19</v>
+      <c r="A19" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>20</v>
+      <c r="A20" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>21</v>
+      <c r="A21" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>22</v>
+      <c r="A22" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>23</v>
+      <c r="A23" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>24</v>
+      <c r="A24" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>25</v>
+      <c r="A25" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>35</v>
+      <c r="A26" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>40</v>
+      <c r="A27" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>